<commit_message>
Eliminados import de otros packages que generaban errores.
</commit_message>
<xml_diff>
--- a/Datos_Pedidos_Test.xlsx
+++ b/Datos_Pedidos_Test.xlsx
@@ -646,12 +646,24 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF66"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -691,7 +703,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="24">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -716,8 +728,60 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -746,6 +810,66 @@
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
     <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF66"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -756,8 +880,8 @@
   </sheetPr>
   <dimension ref="A1:M138"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L19" activeCellId="0" sqref="L19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L17" activeCellId="0" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -935,35 +1059,35 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="n">
+    <row r="6" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="6" t="n">
         <v>20104</v>
       </c>
-      <c r="B6" s="1" t="n">
+      <c r="B6" s="6" t="n">
         <v>1044</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6" s="7" t="n">
         <v>16600</v>
       </c>
-      <c r="F6" s="3" t="n">
+      <c r="F6" s="8" t="n">
         <v>9088500</v>
       </c>
-      <c r="G6" s="4" t="n">
+      <c r="G6" s="9" t="n">
         <v>42015</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="I6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="J6" s="5" t="n">
+      <c r="J6" s="10" t="n">
         <v>6.9</v>
       </c>
     </row>
@@ -999,67 +1123,67 @@
         <v>13.2</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="n">
+    <row r="8" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="6" t="n">
         <v>20106</v>
       </c>
-      <c r="B8" s="1" t="n">
+      <c r="B8" s="6" t="n">
         <v>1049</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="0" t="n">
+      <c r="E8" s="7" t="n">
         <v>10600</v>
       </c>
-      <c r="F8" s="3" t="n">
+      <c r="F8" s="8" t="n">
         <v>6964200</v>
       </c>
-      <c r="G8" s="4" t="n">
+      <c r="G8" s="9" t="n">
         <v>42022</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="I8" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="5" t="n">
+      <c r="J8" s="10" t="n">
         <v>4.4</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="n">
+    <row r="9" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="6" t="n">
         <v>20107</v>
       </c>
-      <c r="B9" s="1" t="n">
+      <c r="B9" s="6" t="n">
         <v>1032</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="0" t="n">
+      <c r="E9" s="7" t="n">
         <v>21100</v>
       </c>
-      <c r="F9" s="3" t="n">
+      <c r="F9" s="8" t="n">
         <v>13092550</v>
       </c>
-      <c r="G9" s="4" t="n">
+      <c r="G9" s="9" t="n">
         <v>42020</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="I9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="5" t="n">
+      <c r="J9" s="10" t="n">
         <v>9.5</v>
       </c>
     </row>
@@ -1255,69 +1379,70 @@
         <v>12.9</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="n">
+    <row r="16" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="6" t="n">
         <v>20114</v>
       </c>
-      <c r="B16" s="1" t="n">
+      <c r="B16" s="6" t="n">
         <v>1014</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="C16" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="0" t="s">
+      <c r="D16" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E16" s="0" t="n">
+      <c r="E16" s="7" t="n">
         <v>22100</v>
       </c>
-      <c r="F16" s="3" t="n">
+      <c r="F16" s="8" t="n">
         <v>12099750</v>
       </c>
-      <c r="G16" s="4" t="n">
+      <c r="G16" s="9" t="n">
         <v>42020</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="H16" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="I16" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="J16" s="5" t="n">
+      <c r="J16" s="10" t="n">
         <v>10.5</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="n">
+    <row r="17" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="6" t="n">
         <v>20115</v>
       </c>
-      <c r="B17" s="1" t="n">
+      <c r="B17" s="6" t="n">
         <v>1034</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="C17" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D17" s="0" t="s">
+      <c r="D17" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="E17" s="0" t="n">
+      <c r="E17" s="7" t="n">
         <v>8900</v>
       </c>
-      <c r="F17" s="3" t="n">
+      <c r="F17" s="8" t="n">
         <v>5522450</v>
       </c>
-      <c r="G17" s="4" t="n">
+      <c r="G17" s="9" t="n">
         <v>42025</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="H17" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="I17" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="J17" s="5" t="n">
+      <c r="J17" s="10" t="n">
         <v>4</v>
       </c>
+      <c r="L17" s="11"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
@@ -1350,7 +1475,7 @@
       <c r="J18" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="M18" s="6"/>
+      <c r="M18" s="12"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
@@ -1512,65 +1637,65 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="n">
+    <row r="24" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="13" t="n">
         <v>24045</v>
       </c>
-      <c r="B24" s="1" t="n">
+      <c r="B24" s="13" t="n">
         <v>1023</v>
       </c>
-      <c r="C24" s="0" t="s">
+      <c r="C24" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="D24" s="0" t="s">
+      <c r="D24" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="E24" s="0" t="n">
+      <c r="E24" s="14" t="n">
         <v>12500</v>
       </c>
-      <c r="F24" s="3" t="n">
+      <c r="F24" s="15" t="n">
         <v>9125000</v>
       </c>
-      <c r="G24" s="4" t="n">
+      <c r="G24" s="16" t="n">
         <v>43198</v>
       </c>
-      <c r="H24" s="1" t="s">
+      <c r="H24" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I24" s="7" t="s">
+      <c r="I24" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="J24" s="2"/>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="n">
+      <c r="J24" s="18"/>
+    </row>
+    <row r="25" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="13" t="n">
         <v>24046</v>
       </c>
-      <c r="B25" s="1" t="n">
+      <c r="B25" s="13" t="n">
         <v>1001</v>
       </c>
-      <c r="C25" s="0" t="s">
+      <c r="C25" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D25" s="0" t="s">
+      <c r="D25" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E25" s="0" t="n">
+      <c r="E25" s="14" t="n">
         <v>19200</v>
       </c>
-      <c r="F25" s="3" t="n">
+      <c r="F25" s="15" t="n">
         <v>11212800</v>
       </c>
-      <c r="G25" s="4" t="n">
+      <c r="G25" s="16" t="n">
         <v>43195</v>
       </c>
-      <c r="H25" s="1" t="s">
+      <c r="H25" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I25" s="1" t="s">
+      <c r="I25" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="J25" s="2"/>
+      <c r="J25" s="18"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
@@ -1602,65 +1727,65 @@
       </c>
       <c r="J26" s="2"/>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="n">
+    <row r="27" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="13" t="n">
         <v>24048</v>
       </c>
-      <c r="B27" s="1" t="n">
+      <c r="B27" s="13" t="n">
         <v>1053</v>
       </c>
-      <c r="C27" s="0" t="s">
+      <c r="C27" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="D27" s="0" t="s">
+      <c r="D27" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="E27" s="0" t="n">
+      <c r="E27" s="14" t="n">
         <v>24000</v>
       </c>
-      <c r="F27" s="3" t="n">
+      <c r="F27" s="15" t="n">
         <v>14016000</v>
       </c>
-      <c r="G27" s="4" t="n">
+      <c r="G27" s="16" t="n">
         <v>43200</v>
       </c>
-      <c r="H27" s="1" t="s">
+      <c r="H27" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I27" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J27" s="2"/>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="n">
+      <c r="I27" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="J27" s="18"/>
+    </row>
+    <row r="28" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="13" t="n">
         <v>24049</v>
       </c>
-      <c r="B28" s="1" t="n">
+      <c r="B28" s="13" t="n">
         <v>1040</v>
       </c>
-      <c r="C28" s="0" t="s">
+      <c r="C28" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="D28" s="0" t="s">
+      <c r="D28" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="E28" s="0" t="n">
+      <c r="E28" s="14" t="n">
         <v>12900</v>
       </c>
-      <c r="F28" s="3" t="n">
+      <c r="F28" s="15" t="n">
         <v>7062750</v>
       </c>
-      <c r="G28" s="4" t="n">
+      <c r="G28" s="16" t="n">
         <v>43200</v>
       </c>
-      <c r="H28" s="1" t="s">
+      <c r="H28" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I28" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J28" s="2"/>
+      <c r="I28" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="J28" s="18"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="n">
@@ -1684,7 +1809,7 @@
       <c r="G29" s="4" t="n">
         <v>43201</v>
       </c>
-      <c r="H29" s="1" t="s">
+      <c r="H29" s="19" t="s">
         <v>12</v>
       </c>
       <c r="I29" s="1" t="s">
@@ -1722,65 +1847,65 @@
       </c>
       <c r="J30" s="2"/>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="n">
+    <row r="31" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="13" t="n">
         <v>24052</v>
       </c>
-      <c r="B31" s="1" t="n">
+      <c r="B31" s="13" t="n">
         <v>1021</v>
       </c>
-      <c r="C31" s="0" t="s">
+      <c r="C31" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="D31" s="0" t="s">
+      <c r="D31" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="E31" s="0" t="n">
+      <c r="E31" s="14" t="n">
         <v>21500</v>
       </c>
-      <c r="F31" s="3" t="n">
+      <c r="F31" s="15" t="n">
         <v>13340750</v>
       </c>
-      <c r="G31" s="4" t="n">
+      <c r="G31" s="16" t="n">
         <v>43201</v>
       </c>
-      <c r="H31" s="1" t="s">
+      <c r="H31" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I31" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J31" s="2"/>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="n">
+      <c r="I31" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="J31" s="18"/>
+    </row>
+    <row r="32" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="13" t="n">
         <v>24053</v>
       </c>
-      <c r="B32" s="1" t="n">
+      <c r="B32" s="13" t="n">
         <v>1047</v>
       </c>
-      <c r="C32" s="0" t="s">
+      <c r="C32" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="0" t="s">
+      <c r="D32" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="E32" s="0" t="n">
+      <c r="E32" s="14" t="n">
         <v>24400</v>
       </c>
-      <c r="F32" s="3" t="n">
+      <c r="F32" s="15" t="n">
         <v>16030800</v>
       </c>
-      <c r="G32" s="4" t="n">
+      <c r="G32" s="16" t="n">
         <v>43200</v>
       </c>
-      <c r="H32" s="1" t="s">
+      <c r="H32" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I32" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J32" s="2"/>
+      <c r="I32" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="J32" s="18"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="n">
@@ -1897,100 +2022,100 @@
       <c r="H36" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I36" s="7" t="s">
+      <c r="I36" s="20" t="s">
         <v>53</v>
       </c>
       <c r="J36" s="2"/>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="1" t="n">
+    <row r="37" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="13" t="n">
         <v>24058</v>
       </c>
-      <c r="B37" s="1" t="n">
+      <c r="B37" s="13" t="n">
         <v>1033</v>
       </c>
-      <c r="C37" s="0" t="s">
+      <c r="C37" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="D37" s="0" t="s">
+      <c r="D37" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="E37" s="0" t="n">
+      <c r="E37" s="14" t="n">
         <v>23200</v>
       </c>
-      <c r="F37" s="3" t="n">
+      <c r="F37" s="15" t="n">
         <v>16936000</v>
       </c>
-      <c r="G37" s="4" t="n">
+      <c r="G37" s="16" t="n">
         <v>43200</v>
       </c>
-      <c r="H37" s="1" t="s">
+      <c r="H37" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I37" s="1" t="s">
+      <c r="I37" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="J37" s="2"/>
-    </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1" t="n">
+      <c r="J37" s="18"/>
+    </row>
+    <row r="38" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="13" t="n">
         <v>24059</v>
       </c>
-      <c r="B38" s="1" t="n">
+      <c r="B38" s="13" t="n">
         <v>1036</v>
       </c>
-      <c r="C38" s="0" t="s">
+      <c r="C38" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="D38" s="0" t="s">
+      <c r="D38" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="E38" s="0" t="n">
+      <c r="E38" s="14" t="n">
         <v>15700</v>
       </c>
-      <c r="F38" s="3" t="n">
+      <c r="F38" s="15" t="n">
         <v>11461000</v>
       </c>
-      <c r="G38" s="4" t="n">
+      <c r="G38" s="16" t="n">
         <v>43201</v>
       </c>
-      <c r="H38" s="1" t="s">
+      <c r="H38" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I38" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J38" s="2"/>
-    </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1" t="n">
+      <c r="I38" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="J38" s="18"/>
+    </row>
+    <row r="39" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="13" t="n">
         <v>24060</v>
       </c>
-      <c r="B39" s="1" t="n">
+      <c r="B39" s="13" t="n">
         <v>1059</v>
       </c>
-      <c r="C39" s="0" t="s">
+      <c r="C39" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D39" s="0" t="s">
+      <c r="D39" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E39" s="0" t="n">
+      <c r="E39" s="14" t="n">
         <v>20100</v>
       </c>
-      <c r="F39" s="3" t="n">
+      <c r="F39" s="15" t="n">
         <v>13205700</v>
       </c>
-      <c r="G39" s="4" t="n">
+      <c r="G39" s="16" t="n">
         <v>43200</v>
       </c>
-      <c r="H39" s="1" t="s">
+      <c r="H39" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I39" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J39" s="2"/>
+      <c r="I39" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="J39" s="18"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="n">
@@ -2022,65 +2147,65 @@
       </c>
       <c r="J40" s="2"/>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1" t="n">
+    <row r="41" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="13" t="n">
         <v>24062</v>
       </c>
-      <c r="B41" s="1" t="n">
+      <c r="B41" s="13" t="n">
         <v>1011</v>
       </c>
-      <c r="C41" s="0" t="s">
+      <c r="C41" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="D41" s="0" t="s">
+      <c r="D41" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="E41" s="0" t="n">
+      <c r="E41" s="14" t="n">
         <v>23600</v>
       </c>
-      <c r="F41" s="3" t="n">
+      <c r="F41" s="15" t="n">
         <v>16366600</v>
       </c>
-      <c r="G41" s="4" t="n">
+      <c r="G41" s="16" t="n">
         <v>43202</v>
       </c>
-      <c r="H41" s="1" t="s">
+      <c r="H41" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I41" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J41" s="2"/>
-    </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="1" t="n">
+      <c r="I41" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="J41" s="18"/>
+    </row>
+    <row r="42" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="13" t="n">
         <v>24063</v>
       </c>
-      <c r="B42" s="1" t="n">
+      <c r="B42" s="13" t="n">
         <v>1024</v>
       </c>
-      <c r="C42" s="0" t="s">
+      <c r="C42" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="D42" s="0" t="s">
+      <c r="D42" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="E42" s="0" t="n">
+      <c r="E42" s="14" t="n">
         <v>24300</v>
       </c>
-      <c r="F42" s="3" t="n">
+      <c r="F42" s="15" t="n">
         <v>13304250</v>
       </c>
-      <c r="G42" s="4" t="n">
+      <c r="G42" s="16" t="n">
         <v>43200</v>
       </c>
-      <c r="H42" s="1" t="s">
+      <c r="H42" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I42" s="1" t="s">
+      <c r="I42" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="J42" s="2"/>
+      <c r="J42" s="18"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="n">
@@ -2112,35 +2237,35 @@
       </c>
       <c r="J43" s="2"/>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="1" t="n">
+    <row r="44" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="13" t="n">
         <v>24065</v>
       </c>
-      <c r="B44" s="1" t="n">
+      <c r="B44" s="13" t="n">
         <v>1002</v>
       </c>
-      <c r="C44" s="0" t="s">
+      <c r="C44" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="D44" s="0" t="s">
+      <c r="D44" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="E44" s="0" t="n">
+      <c r="E44" s="14" t="n">
         <v>9000</v>
       </c>
-      <c r="F44" s="3" t="n">
+      <c r="F44" s="15" t="n">
         <v>5256000</v>
       </c>
-      <c r="G44" s="4" t="n">
+      <c r="G44" s="16" t="n">
         <v>43200</v>
       </c>
-      <c r="H44" s="1" t="s">
+      <c r="H44" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I44" s="1" t="s">
+      <c r="I44" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="J44" s="2"/>
+      <c r="J44" s="18"/>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="n">
@@ -2232,65 +2357,65 @@
       </c>
       <c r="J47" s="2"/>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="1" t="n">
+    <row r="48" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="13" t="n">
         <v>24069</v>
       </c>
-      <c r="B48" s="1" t="n">
+      <c r="B48" s="13" t="n">
         <v>1061</v>
       </c>
-      <c r="C48" s="0" t="s">
+      <c r="C48" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="D48" s="0" t="s">
+      <c r="D48" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="E48" s="0" t="n">
+      <c r="E48" s="14" t="n">
         <v>10000</v>
       </c>
-      <c r="F48" s="3" t="n">
+      <c r="F48" s="15" t="n">
         <v>6570000</v>
       </c>
-      <c r="G48" s="4" t="n">
+      <c r="G48" s="16" t="n">
         <v>43200</v>
       </c>
-      <c r="H48" s="1" t="s">
+      <c r="H48" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I48" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J48" s="2"/>
-    </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="1" t="n">
+      <c r="I48" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="J48" s="18"/>
+    </row>
+    <row r="49" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="13" t="n">
         <v>24070</v>
       </c>
-      <c r="B49" s="1" t="n">
+      <c r="B49" s="13" t="n">
         <v>1028</v>
       </c>
-      <c r="C49" s="0" t="s">
+      <c r="C49" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="D49" s="0" t="s">
+      <c r="D49" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="E49" s="0" t="n">
+      <c r="E49" s="14" t="n">
         <v>19800</v>
       </c>
-      <c r="F49" s="3" t="n">
+      <c r="F49" s="15" t="n">
         <v>10840500</v>
       </c>
-      <c r="G49" s="4" t="n">
+      <c r="G49" s="16" t="n">
         <v>43202</v>
       </c>
-      <c r="H49" s="1" t="s">
+      <c r="H49" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I49" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J49" s="2"/>
+      <c r="I49" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="J49" s="18"/>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="n">
@@ -2322,35 +2447,35 @@
       </c>
       <c r="J50" s="2"/>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="1" t="n">
+    <row r="51" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="13" t="n">
         <v>24072</v>
       </c>
-      <c r="B51" s="1" t="n">
+      <c r="B51" s="13" t="n">
         <v>1016</v>
       </c>
-      <c r="C51" s="0" t="s">
+      <c r="C51" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="D51" s="0" t="s">
+      <c r="D51" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="E51" s="0" t="n">
+      <c r="E51" s="14" t="n">
         <v>19000</v>
       </c>
-      <c r="F51" s="3" t="n">
+      <c r="F51" s="15" t="n">
         <v>10402500</v>
       </c>
-      <c r="G51" s="4" t="n">
+      <c r="G51" s="16" t="n">
         <v>43202</v>
       </c>
-      <c r="H51" s="1" t="s">
+      <c r="H51" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I51" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J51" s="2"/>
+      <c r="I51" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="J51" s="18"/>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="n">
@@ -2412,35 +2537,35 @@
       </c>
       <c r="J53" s="2"/>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="1" t="n">
+    <row r="54" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="13" t="n">
         <v>24075</v>
       </c>
-      <c r="B54" s="1" t="n">
+      <c r="B54" s="13" t="n">
         <v>1001</v>
       </c>
-      <c r="C54" s="0" t="s">
+      <c r="C54" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D54" s="0" t="s">
+      <c r="D54" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="E54" s="0" t="n">
+      <c r="E54" s="14" t="n">
         <v>21200</v>
       </c>
-      <c r="F54" s="3" t="n">
+      <c r="F54" s="15" t="n">
         <v>15476000</v>
       </c>
-      <c r="G54" s="4" t="n">
+      <c r="G54" s="16" t="n">
         <v>43203</v>
       </c>
-      <c r="H54" s="1" t="s">
+      <c r="H54" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I54" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J54" s="2"/>
+      <c r="I54" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="J54" s="18"/>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="n">
@@ -2502,65 +2627,65 @@
       </c>
       <c r="J56" s="2"/>
     </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="1" t="n">
+    <row r="57" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="13" t="n">
         <v>24078</v>
       </c>
-      <c r="B57" s="1" t="n">
+      <c r="B57" s="13" t="n">
         <v>1034</v>
       </c>
-      <c r="C57" s="0" t="s">
+      <c r="C57" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="D57" s="0" t="s">
+      <c r="D57" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="E57" s="0" t="n">
+      <c r="E57" s="14" t="n">
         <v>9500</v>
       </c>
-      <c r="F57" s="3" t="n">
+      <c r="F57" s="15" t="n">
         <v>5548000</v>
       </c>
-      <c r="G57" s="4" t="n">
+      <c r="G57" s="16" t="n">
         <v>43203</v>
       </c>
-      <c r="H57" s="1" t="s">
+      <c r="H57" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I57" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J57" s="2"/>
-    </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="1" t="n">
+      <c r="I57" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="J57" s="18"/>
+    </row>
+    <row r="58" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="13" t="n">
         <v>24079</v>
       </c>
-      <c r="B58" s="1" t="n">
+      <c r="B58" s="13" t="n">
         <v>1009</v>
       </c>
-      <c r="C58" s="0" t="s">
+      <c r="C58" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D58" s="0" t="s">
+      <c r="D58" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="E58" s="0" t="n">
+      <c r="E58" s="14" t="n">
         <v>21400</v>
       </c>
-      <c r="F58" s="3" t="n">
+      <c r="F58" s="15" t="n">
         <v>14059800</v>
       </c>
-      <c r="G58" s="4" t="n">
+      <c r="G58" s="16" t="n">
         <v>43202</v>
       </c>
-      <c r="H58" s="1" t="s">
+      <c r="H58" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I58" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J58" s="2"/>
+      <c r="I58" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="J58" s="18"/>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="n">
@@ -2622,35 +2747,35 @@
       </c>
       <c r="J60" s="2"/>
     </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="1" t="n">
+    <row r="61" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="13" t="n">
         <v>24082</v>
       </c>
-      <c r="B61" s="1" t="n">
+      <c r="B61" s="13" t="n">
         <v>1005</v>
       </c>
-      <c r="C61" s="0" t="s">
+      <c r="C61" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="D61" s="0" t="s">
+      <c r="D61" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="E61" s="0" t="n">
+      <c r="E61" s="14" t="n">
         <v>24300</v>
       </c>
-      <c r="F61" s="3" t="n">
+      <c r="F61" s="15" t="n">
         <v>13304250</v>
       </c>
-      <c r="G61" s="4" t="n">
+      <c r="G61" s="16" t="n">
         <v>43204</v>
       </c>
-      <c r="H61" s="1" t="s">
+      <c r="H61" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I61" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J61" s="2"/>
+      <c r="I61" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="J61" s="18"/>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="n">
@@ -2682,35 +2807,35 @@
       </c>
       <c r="J62" s="2"/>
     </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="1" t="n">
+    <row r="63" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="13" t="n">
         <v>24084</v>
       </c>
-      <c r="B63" s="1" t="n">
+      <c r="B63" s="13" t="n">
         <v>1025</v>
       </c>
-      <c r="C63" s="0" t="s">
+      <c r="C63" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="D63" s="0" t="s">
+      <c r="D63" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="E63" s="0" t="n">
+      <c r="E63" s="14" t="n">
         <v>14700</v>
       </c>
-      <c r="F63" s="3" t="n">
+      <c r="F63" s="15" t="n">
         <v>9121350</v>
       </c>
-      <c r="G63" s="4" t="n">
+      <c r="G63" s="16" t="n">
         <v>43204</v>
       </c>
-      <c r="H63" s="1" t="s">
+      <c r="H63" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I63" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J63" s="2"/>
+      <c r="I63" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="J63" s="18"/>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="n">
@@ -2832,35 +2957,35 @@
       </c>
       <c r="J67" s="2"/>
     </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="1" t="n">
+    <row r="68" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="13" t="n">
         <v>24089</v>
       </c>
-      <c r="B68" s="1" t="n">
+      <c r="B68" s="13" t="n">
         <v>1030</v>
       </c>
-      <c r="C68" s="0" t="s">
+      <c r="C68" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="D68" s="0" t="s">
+      <c r="D68" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="E68" s="0" t="n">
+      <c r="E68" s="14" t="n">
         <v>22100</v>
       </c>
-      <c r="F68" s="3" t="n">
+      <c r="F68" s="15" t="n">
         <v>15326350</v>
       </c>
-      <c r="G68" s="4" t="n">
+      <c r="G68" s="16" t="n">
         <v>43207</v>
       </c>
-      <c r="H68" s="1" t="s">
+      <c r="H68" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I68" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J68" s="2"/>
+      <c r="I68" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="J68" s="18"/>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="n">
@@ -2892,35 +3017,35 @@
       </c>
       <c r="J69" s="2"/>
     </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="1" t="n">
+    <row r="70" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="13" t="n">
         <v>24091</v>
       </c>
-      <c r="B70" s="1" t="n">
+      <c r="B70" s="13" t="n">
         <v>1017</v>
       </c>
-      <c r="C70" s="0" t="s">
+      <c r="C70" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="D70" s="0" t="s">
+      <c r="D70" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="E70" s="0" t="n">
+      <c r="E70" s="14" t="n">
         <v>20800</v>
       </c>
-      <c r="F70" s="3" t="n">
+      <c r="F70" s="15" t="n">
         <v>13665600</v>
       </c>
-      <c r="G70" s="4" t="n">
+      <c r="G70" s="16" t="n">
         <v>43205</v>
       </c>
-      <c r="H70" s="1" t="s">
+      <c r="H70" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I70" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J70" s="2"/>
+      <c r="I70" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="J70" s="18"/>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="n">
@@ -2952,35 +3077,35 @@
       </c>
       <c r="J71" s="2"/>
     </row>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="1" t="n">
+    <row r="72" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="13" t="n">
         <v>24093</v>
       </c>
-      <c r="B72" s="1" t="n">
+      <c r="B72" s="13" t="n">
         <v>1031</v>
       </c>
-      <c r="C72" s="0" t="s">
+      <c r="C72" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="D72" s="0" t="s">
+      <c r="D72" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="E72" s="0" t="n">
+      <c r="E72" s="14" t="n">
         <v>8300</v>
       </c>
-      <c r="F72" s="3" t="n">
+      <c r="F72" s="15" t="n">
         <v>4847200</v>
       </c>
-      <c r="G72" s="4" t="n">
+      <c r="G72" s="16" t="n">
         <v>43204</v>
       </c>
-      <c r="H72" s="1" t="s">
+      <c r="H72" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I72" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J72" s="2"/>
+      <c r="I72" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="J72" s="18"/>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="n">
@@ -3042,35 +3167,35 @@
       </c>
       <c r="J74" s="2"/>
     </row>
-    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="1" t="n">
+    <row r="75" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="13" t="n">
         <v>24096</v>
       </c>
-      <c r="B75" s="1" t="n">
+      <c r="B75" s="13" t="n">
         <v>1039</v>
       </c>
-      <c r="C75" s="0" t="s">
+      <c r="C75" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="D75" s="0" t="s">
+      <c r="D75" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="E75" s="0" t="n">
+      <c r="E75" s="14" t="n">
         <v>12400</v>
       </c>
-      <c r="F75" s="3" t="n">
+      <c r="F75" s="15" t="n">
         <v>9052000</v>
       </c>
-      <c r="G75" s="4" t="n">
+      <c r="G75" s="16" t="n">
         <v>43206</v>
       </c>
-      <c r="H75" s="1" t="s">
+      <c r="H75" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I75" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J75" s="2"/>
+      <c r="I75" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="J75" s="18"/>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="n">
@@ -3162,35 +3287,35 @@
       </c>
       <c r="J78" s="2"/>
     </row>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="1" t="n">
+    <row r="79" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="13" t="n">
         <v>24100</v>
       </c>
-      <c r="B79" s="1" t="n">
+      <c r="B79" s="13" t="n">
         <v>1028</v>
       </c>
-      <c r="C79" s="0" t="s">
+      <c r="C79" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="D79" s="0" t="s">
+      <c r="D79" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="E79" s="0" t="n">
+      <c r="E79" s="14" t="n">
         <v>21800</v>
       </c>
-      <c r="F79" s="3" t="n">
+      <c r="F79" s="15" t="n">
         <v>13526900</v>
       </c>
-      <c r="G79" s="4" t="n">
+      <c r="G79" s="16" t="n">
         <v>43206</v>
       </c>
-      <c r="H79" s="1" t="s">
+      <c r="H79" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I79" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J79" s="2"/>
+      <c r="I79" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="J79" s="18"/>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="n">
@@ -3252,65 +3377,65 @@
       </c>
       <c r="J81" s="2"/>
     </row>
-    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="1" t="n">
+    <row r="82" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="13" t="n">
         <v>24103</v>
       </c>
-      <c r="B82" s="1" t="n">
+      <c r="B82" s="13" t="n">
         <v>1026</v>
       </c>
-      <c r="C82" s="0" t="s">
+      <c r="C82" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="D82" s="0" t="s">
+      <c r="D82" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="E82" s="0" t="n">
+      <c r="E82" s="14" t="n">
         <v>21600</v>
       </c>
-      <c r="F82" s="3" t="n">
+      <c r="F82" s="15" t="n">
         <v>15768000</v>
       </c>
-      <c r="G82" s="4" t="n">
+      <c r="G82" s="16" t="n">
         <v>43207</v>
       </c>
-      <c r="H82" s="1" t="s">
+      <c r="H82" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I82" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J82" s="2"/>
-    </row>
-    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="1" t="n">
+      <c r="I82" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="J82" s="18"/>
+    </row>
+    <row r="83" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="13" t="n">
         <v>24104</v>
       </c>
-      <c r="B83" s="1" t="n">
+      <c r="B83" s="13" t="n">
         <v>1025</v>
       </c>
-      <c r="C83" s="0" t="s">
+      <c r="C83" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="D83" s="0" t="s">
+      <c r="D83" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="E83" s="0" t="n">
+      <c r="E83" s="14" t="n">
         <v>13600</v>
       </c>
-      <c r="F83" s="3" t="n">
+      <c r="F83" s="15" t="n">
         <v>7942400</v>
       </c>
-      <c r="G83" s="4" t="n">
+      <c r="G83" s="16" t="n">
         <v>43206</v>
       </c>
-      <c r="H83" s="1" t="s">
+      <c r="H83" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I83" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J83" s="2"/>
+      <c r="I83" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="J83" s="18"/>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="n">
@@ -3372,185 +3497,185 @@
       </c>
       <c r="J85" s="2"/>
     </row>
-    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="1" t="n">
+    <row r="86" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="13" t="n">
         <v>24107</v>
       </c>
-      <c r="B86" s="1" t="n">
+      <c r="B86" s="13" t="n">
         <v>1040</v>
       </c>
-      <c r="C86" s="0" t="s">
+      <c r="C86" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="D86" s="0" t="s">
+      <c r="D86" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="E86" s="0" t="n">
+      <c r="E86" s="14" t="n">
         <v>16700</v>
       </c>
-      <c r="F86" s="3" t="n">
+      <c r="F86" s="15" t="n">
         <v>10971900</v>
       </c>
-      <c r="G86" s="4" t="n">
+      <c r="G86" s="16" t="n">
         <v>43205</v>
       </c>
-      <c r="H86" s="1" t="s">
+      <c r="H86" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I86" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J86" s="2"/>
-    </row>
-    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="1" t="n">
+      <c r="I86" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="J86" s="18"/>
+    </row>
+    <row r="87" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="13" t="n">
         <v>24108</v>
       </c>
-      <c r="B87" s="1" t="n">
+      <c r="B87" s="13" t="n">
         <v>1042</v>
       </c>
-      <c r="C87" s="0" t="s">
+      <c r="C87" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="D87" s="0" t="s">
+      <c r="D87" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="E87" s="0" t="n">
+      <c r="E87" s="14" t="n">
         <v>22500</v>
       </c>
-      <c r="F87" s="3" t="n">
+      <c r="F87" s="15" t="n">
         <v>12318750</v>
       </c>
-      <c r="G87" s="4" t="n">
+      <c r="G87" s="16" t="n">
         <v>43207</v>
       </c>
-      <c r="H87" s="1" t="s">
+      <c r="H87" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I87" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J87" s="2"/>
-    </row>
-    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="1" t="n">
+      <c r="I87" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="J87" s="18"/>
+    </row>
+    <row r="88" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="13" t="n">
         <v>24109</v>
       </c>
-      <c r="B88" s="1" t="n">
+      <c r="B88" s="13" t="n">
         <v>1048</v>
       </c>
-      <c r="C88" s="0" t="s">
+      <c r="C88" s="14" t="s">
         <v>141</v>
       </c>
-      <c r="D88" s="0" t="s">
+      <c r="D88" s="14" t="s">
         <v>142</v>
       </c>
-      <c r="E88" s="0" t="n">
+      <c r="E88" s="14" t="n">
         <v>9200</v>
       </c>
-      <c r="F88" s="3" t="n">
+      <c r="F88" s="15" t="n">
         <v>6044400</v>
       </c>
-      <c r="G88" s="4" t="n">
+      <c r="G88" s="16" t="n">
         <v>43210</v>
       </c>
-      <c r="H88" s="1" t="s">
+      <c r="H88" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I88" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J88" s="2"/>
-    </row>
-    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="1" t="n">
+      <c r="I88" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="J88" s="18"/>
+    </row>
+    <row r="89" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="13" t="n">
         <v>24110</v>
       </c>
-      <c r="B89" s="1" t="n">
+      <c r="B89" s="13" t="n">
         <v>1019</v>
       </c>
-      <c r="C89" s="0" t="s">
+      <c r="C89" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="D89" s="0" t="s">
+      <c r="D89" s="14" t="s">
         <v>143</v>
       </c>
-      <c r="E89" s="0" t="n">
+      <c r="E89" s="14" t="n">
         <v>18900</v>
       </c>
-      <c r="F89" s="3" t="n">
+      <c r="F89" s="15" t="n">
         <v>11727450</v>
       </c>
-      <c r="G89" s="4" t="n">
+      <c r="G89" s="16" t="n">
         <v>43208</v>
       </c>
-      <c r="H89" s="1" t="s">
+      <c r="H89" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I89" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J89" s="2"/>
-    </row>
-    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="1" t="n">
+      <c r="I89" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="J89" s="18"/>
+    </row>
+    <row r="90" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="13" t="n">
         <v>24111</v>
       </c>
-      <c r="B90" s="1" t="n">
+      <c r="B90" s="13" t="n">
         <v>1048</v>
       </c>
-      <c r="C90" s="0" t="s">
+      <c r="C90" s="14" t="s">
         <v>141</v>
       </c>
-      <c r="D90" s="0" t="s">
+      <c r="D90" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="E90" s="0" t="n">
+      <c r="E90" s="14" t="n">
         <v>17100</v>
       </c>
-      <c r="F90" s="3" t="n">
+      <c r="F90" s="15" t="n">
         <v>9986400</v>
       </c>
-      <c r="G90" s="4" t="n">
+      <c r="G90" s="16" t="n">
         <v>43239</v>
       </c>
-      <c r="H90" s="1" t="s">
+      <c r="H90" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I90" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J90" s="2"/>
-    </row>
-    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="1" t="n">
+      <c r="I90" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="J90" s="18"/>
+    </row>
+    <row r="91" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="13" t="n">
         <v>24112</v>
       </c>
-      <c r="B91" s="1" t="n">
+      <c r="B91" s="13" t="n">
         <v>1013</v>
       </c>
-      <c r="C91" s="0" t="s">
+      <c r="C91" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="D91" s="0" t="s">
+      <c r="D91" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="E91" s="0" t="n">
+      <c r="E91" s="14" t="n">
         <v>11600</v>
       </c>
-      <c r="F91" s="3" t="n">
+      <c r="F91" s="15" t="n">
         <v>8468000</v>
       </c>
-      <c r="G91" s="4" t="n">
+      <c r="G91" s="16" t="n">
         <v>43205</v>
       </c>
-      <c r="H91" s="1" t="s">
+      <c r="H91" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I91" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J91" s="2"/>
+      <c r="I91" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="J91" s="18"/>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="n">
@@ -3672,35 +3797,35 @@
       </c>
       <c r="J95" s="2"/>
     </row>
-    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="1" t="n">
+    <row r="96" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="13" t="n">
         <v>24117</v>
       </c>
-      <c r="B96" s="1" t="n">
+      <c r="B96" s="13" t="n">
         <v>1025</v>
       </c>
-      <c r="C96" s="0" t="s">
+      <c r="C96" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="D96" s="0" t="s">
+      <c r="D96" s="14" t="s">
         <v>151</v>
       </c>
-      <c r="E96" s="0" t="n">
+      <c r="E96" s="14" t="n">
         <v>8200</v>
       </c>
-      <c r="F96" s="3" t="n">
+      <c r="F96" s="15" t="n">
         <v>5986000</v>
       </c>
-      <c r="G96" s="4" t="n">
+      <c r="G96" s="16" t="n">
         <v>43212</v>
       </c>
-      <c r="H96" s="1" t="s">
+      <c r="H96" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I96" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J96" s="2"/>
+      <c r="I96" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="J96" s="18"/>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="n">
@@ -3822,35 +3947,35 @@
       </c>
       <c r="J100" s="2"/>
     </row>
-    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="1" t="n">
+    <row r="101" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="13" t="n">
         <v>24122</v>
       </c>
-      <c r="B101" s="1" t="n">
+      <c r="B101" s="13" t="n">
         <v>1018</v>
       </c>
-      <c r="C101" s="0" t="s">
+      <c r="C101" s="14" t="s">
         <v>156</v>
       </c>
-      <c r="D101" s="0" t="s">
+      <c r="D101" s="14" t="s">
         <v>157</v>
       </c>
-      <c r="E101" s="0" t="n">
+      <c r="E101" s="14" t="n">
         <v>17400</v>
       </c>
-      <c r="F101" s="3" t="n">
+      <c r="F101" s="15" t="n">
         <v>12702000</v>
       </c>
-      <c r="G101" s="4" t="n">
+      <c r="G101" s="16" t="n">
         <v>43212</v>
       </c>
-      <c r="H101" s="1" t="s">
+      <c r="H101" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I101" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J101" s="2"/>
+      <c r="I101" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="J101" s="18"/>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="1" t="n">
@@ -3912,35 +4037,35 @@
       </c>
       <c r="J103" s="2"/>
     </row>
-    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="1" t="n">
+    <row r="104" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="13" t="n">
         <v>24125</v>
       </c>
-      <c r="B104" s="1" t="n">
+      <c r="B104" s="13" t="n">
         <v>1049</v>
       </c>
-      <c r="C104" s="0" t="s">
+      <c r="C104" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D104" s="0" t="s">
+      <c r="D104" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="E104" s="0" t="n">
+      <c r="E104" s="14" t="n">
         <v>15600</v>
       </c>
-      <c r="F104" s="3" t="n">
+      <c r="F104" s="15" t="n">
         <v>9679800</v>
       </c>
-      <c r="G104" s="4" t="n">
+      <c r="G104" s="16" t="n">
         <v>43207</v>
       </c>
-      <c r="H104" s="1" t="s">
+      <c r="H104" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I104" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J104" s="2"/>
+      <c r="I104" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="J104" s="18"/>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="1" t="n">
@@ -4002,35 +4127,35 @@
       </c>
       <c r="J106" s="2"/>
     </row>
-    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="1" t="n">
+    <row r="107" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="13" t="n">
         <v>24128</v>
       </c>
-      <c r="B107" s="1" t="n">
+      <c r="B107" s="13" t="n">
         <v>1047</v>
       </c>
-      <c r="C107" s="0" t="s">
+      <c r="C107" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="D107" s="0" t="s">
+      <c r="D107" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="E107" s="0" t="n">
+      <c r="E107" s="14" t="n">
         <v>20600</v>
       </c>
-      <c r="F107" s="3" t="n">
+      <c r="F107" s="15" t="n">
         <v>11278500</v>
       </c>
-      <c r="G107" s="4" t="n">
+      <c r="G107" s="16" t="n">
         <v>43213</v>
       </c>
-      <c r="H107" s="1" t="s">
+      <c r="H107" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I107" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J107" s="2"/>
+      <c r="I107" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="J107" s="18"/>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="1" t="n">
@@ -4242,35 +4367,35 @@
       </c>
       <c r="J114" s="2"/>
     </row>
-    <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="1" t="n">
+    <row r="115" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="13" t="n">
         <v>24136</v>
       </c>
-      <c r="B115" s="1" t="n">
+      <c r="B115" s="13" t="n">
         <v>1059</v>
       </c>
-      <c r="C115" s="0" t="s">
+      <c r="C115" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D115" s="0" t="s">
+      <c r="D115" s="14" t="s">
         <v>172</v>
       </c>
-      <c r="E115" s="0" t="n">
+      <c r="E115" s="14" t="n">
         <v>10900</v>
       </c>
-      <c r="F115" s="3" t="n">
+      <c r="F115" s="15" t="n">
         <v>6365600</v>
       </c>
-      <c r="G115" s="4" t="n">
+      <c r="G115" s="16" t="n">
         <v>43210</v>
       </c>
-      <c r="H115" s="1" t="s">
+      <c r="H115" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I115" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J115" s="2"/>
+      <c r="I115" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="J115" s="18"/>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="1" t="n">
@@ -4602,35 +4727,35 @@
       </c>
       <c r="J126" s="2"/>
     </row>
-    <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="1" t="n">
+    <row r="127" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="13" t="n">
         <v>24148</v>
       </c>
-      <c r="B127" s="1" t="n">
+      <c r="B127" s="13" t="n">
         <v>1017</v>
       </c>
-      <c r="C127" s="0" t="s">
+      <c r="C127" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="D127" s="0" t="s">
+      <c r="D127" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="E127" s="0" t="n">
+      <c r="E127" s="14" t="n">
         <v>13900</v>
       </c>
-      <c r="F127" s="3" t="n">
+      <c r="F127" s="15" t="n">
         <v>10147000</v>
       </c>
-      <c r="G127" s="4" t="n">
+      <c r="G127" s="16" t="n">
         <v>43230</v>
       </c>
-      <c r="H127" s="1" t="s">
+      <c r="H127" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I127" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J127" s="2"/>
+      <c r="I127" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="J127" s="18"/>
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="1" t="n">
@@ -4782,35 +4907,35 @@
       </c>
       <c r="J132" s="2"/>
     </row>
-    <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="1" t="n">
+    <row r="133" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="13" t="n">
         <v>24154</v>
       </c>
-      <c r="B133" s="1" t="n">
+      <c r="B133" s="13" t="n">
         <v>1045</v>
       </c>
-      <c r="C133" s="0" t="s">
+      <c r="C133" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="D133" s="0" t="s">
+      <c r="D133" s="14" t="s">
         <v>187</v>
       </c>
-      <c r="E133" s="0" t="n">
+      <c r="E133" s="14" t="n">
         <v>24600</v>
       </c>
-      <c r="F133" s="3" t="n">
+      <c r="F133" s="15" t="n">
         <v>17060100</v>
       </c>
-      <c r="G133" s="4" t="n">
+      <c r="G133" s="16" t="n">
         <v>43231</v>
       </c>
-      <c r="H133" s="1" t="s">
+      <c r="H133" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I133" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J133" s="2"/>
+      <c r="I133" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="J133" s="18"/>
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="1" t="n">
@@ -4936,16 +5061,16 @@
       <c r="A138" s="1" t="n">
         <v>24159</v>
       </c>
-      <c r="B138" s="8" t="n">
+      <c r="B138" s="21" t="n">
         <v>1059</v>
       </c>
-      <c r="C138" s="9" t="s">
+      <c r="C138" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="D138" s="9" t="s">
+      <c r="D138" s="22" t="s">
         <v>191</v>
       </c>
-      <c r="E138" s="9" t="n">
+      <c r="E138" s="22" t="n">
         <v>8100</v>
       </c>
       <c r="F138" s="3" t="n">
@@ -4960,7 +5085,7 @@
       <c r="I138" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="J138" s="10"/>
+      <c r="J138" s="23"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>